<commit_message>
Added new IPA script
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IPAIAM.xlsx
+++ b/src/test/resources/xls/IPAIAM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="17235" windowHeight="6210"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="57">
   <si>
     <t>TCID</t>
   </si>
@@ -179,13 +179,22 @@
   </si>
   <si>
     <t>OPQA-4180||OPQA-4177</t>
+  </si>
+  <si>
+    <t>IPAIAM0057</t>
+  </si>
+  <si>
+    <t>OPQA-4525||OPQA-4526||OPQA-4527</t>
+  </si>
+  <si>
+    <t>Verify that the STeAM Step Up Auth Modal should be presented to the user without a pre-populated email address when user has a valid Neon session token and is navigating within the same browser window.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -366,6 +375,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -400,6 +410,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -575,14 +586,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="44.140625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -591,7 +602,7 @@
     <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -608,7 +619,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="120">
+    <row r="2" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>36</v>
       </c>
@@ -623,7 +634,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="90">
+    <row r="3" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>37</v>
       </c>
@@ -638,7 +649,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="75">
+    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>38</v>
       </c>
@@ -653,7 +664,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="90">
+    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>39</v>
       </c>
@@ -668,7 +679,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="45">
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>40</v>
       </c>
@@ -683,7 +694,7 @@
       </c>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:5" ht="75">
+    <row r="7" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>41</v>
       </c>
@@ -698,7 +709,7 @@
       </c>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:5" ht="90">
+    <row r="8" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>42</v>
       </c>
@@ -713,7 +724,7 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" ht="45">
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>43</v>
       </c>
@@ -728,7 +739,7 @@
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" ht="30">
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>44</v>
       </c>
@@ -743,7 +754,7 @@
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" ht="30">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>45</v>
       </c>
@@ -758,7 +769,7 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" ht="45">
+    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>46</v>
       </c>
@@ -773,7 +784,7 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" ht="120">
+    <row r="13" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>47</v>
       </c>
@@ -788,7 +799,7 @@
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" ht="75">
+    <row r="14" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>48</v>
       </c>
@@ -803,7 +814,7 @@
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" ht="45">
+    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>49</v>
       </c>
@@ -818,7 +829,7 @@
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" ht="45">
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>50</v>
       </c>
@@ -833,7 +844,7 @@
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" ht="45">
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>51</v>
       </c>
@@ -847,6 +858,21 @@
         <v>52</v>
       </c>
       <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -859,24 +885,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new IPA scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IPAIAM.xlsx
+++ b/src/test/resources/xls/IPAIAM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="66">
   <si>
     <t>TCID</t>
   </si>
@@ -197,6 +197,24 @@
   </si>
   <si>
     <t>IPAIAM0058</t>
+  </si>
+  <si>
+    <t>OPQA-4561</t>
+  </si>
+  <si>
+    <t>Verify that STeAM account locked message sholud be displayed in an overlay as below " Your account has been locked for 30 minutes due to too many failed attempts." &lt;Okay&gt;</t>
+  </si>
+  <si>
+    <t>OPQA-4563</t>
+  </si>
+  <si>
+    <t>Verify that when STeAM account email is in an unverified status,below error message should be displayed Your email address has not yet been verified.</t>
+  </si>
+  <si>
+    <t>IPAIAM0059</t>
+  </si>
+  <si>
+    <t>IPAIAM0060</t>
   </si>
 </sst>
 </file>
@@ -596,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,6 +915,36 @@
         <v>52</v>
       </c>
       <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
adding IPA100 to IPAIAM suite
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IPAIAM.xlsx
+++ b/src/test/resources/xls/IPAIAM.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sb94731\git\Newworspace17oct\src\test\resources\xls\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="17235" windowHeight="6210"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="71">
   <si>
     <t>TCID</t>
   </si>
@@ -221,16 +226,41 @@
   </si>
   <si>
     <t>Verify that STeAM account locked message sholud be displayed in an overlay as below " Your account has been locked for 30 minutes due to too many failed attempts." &lt;Okay&gt;||Verify that STeAM account is suspended message sholud be displayed in an overlay as below " Your account has been evicted. To get help, please email ProjectNeon@tr.com. &lt;Okay&gt;</t>
+  </si>
+  <si>
+    <t>OPQA-1934||
+OPQA-1935&amp;OPQA-3687||
+OPQA-4230||OPQA-4229||
+OPQA-4231||OPQA-4232||
+OPQA-4636||OPQA-4261||
+OPQA-4244||OPQA-4264||
+OPQA-4265||OPQA-4237||
+OPQA-4239||OPQA-4240||
+OPQA-4246||OPQA-4248||
+OPQA-4252</t>
+  </si>
+  <si>
+    <t>Verify that Forgot your password? Link is clickable on NEON Landing page and End note landing page||Verify that the system is navigating to Forgot Password page or not|| after clicking on Forgot your password? Link&amp;Verify that||the system should support a ENW password reset workflow with the following configurations||Verify that system should not inform user that entered email is not found.||Verify that user should be able to enter email address in Forgot password page.||Verify that  forget password service should send a forgot password email when the email entered is registered in the system||Verify that the platform password reset service should send a platform forget password email with branding that corresponds with the originating application as per wireframe||Verify that When the password reset token in the email is valid|| upon clicking the password reset link in the the platform forget password email|| the user shall be taken to the External Password Reset Page||Verify that External Password Reset Page should have a new password field where the user enters their new password.||Verify that when reset Password Token already used user should be taken to sign in screen||Verify that upon successful submission of a password change|| The user should receive a password change confirmation email to the user's primary email address with branding that corresponds with the application that the user completed the password change||Verify that the password change confirmation email should reference the fact that credentials are shared across all products.||Verify that when the password reset token in the email is expired or already used|| upon clicking the password reset link in the the platform forget password email|| the user should be taken to the External Invalid Password Reset Token Page.||Verify that the email address on the External Invalid Password Reset Token Page should be pre-populated with the email address that matches the email that the forgot password email was sent.||Verify that user who clicks the submit button on the the External Invalid Password Reset Token page|| should be taken to the target application sign in page.||Verify that when Email address is known from password reset token||error message 'The email address is prepopulated.' should be displayed and email address field should be editable||Verify that when Email address is not known from password reset token||email address field should be blank and user should be able to enter any email address||Verify that error message Please enter a valid email address.should be displayed in red color when user enters email address in wrong format</t>
+  </si>
+  <si>
+    <t>IPAIAM100</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -277,7 +307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -286,6 +316,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -376,7 +409,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -411,7 +444,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -620,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,6 +999,21 @@
         <v>52</v>
       </c>
       <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
New Script : IPAIAM0006
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IPAIAM.xlsx
+++ b/src/test/resources/xls/IPAIAM.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sb94731\git\Newworspace17oct\src\test\resources\xls\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="17235" windowHeight="6210"/>
   </bookViews>
@@ -16,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="74">
   <si>
     <t>TCID</t>
   </si>
@@ -244,6 +239,15 @@
   </si>
   <si>
     <t>IPAIAM100</t>
+  </si>
+  <si>
+    <t>IPAIAM0006</t>
+  </si>
+  <si>
+    <t>OPQA-4531||OPQA-4533||OPQA-4547||OPQA-4550</t>
+  </si>
+  <si>
+    <t>Verify that the new STeAM step up authentication modal should include a link to initiate the EndNote supported forgot password flow. || Verify that the "Sign in to Target Druggability" modal should match with wireframe || Verify that the target application product overview page should be opened in a separate browser window when User clicks "Learn more" in any of the Step up related messages/modals.||Verify that the DRA\IPA application overview page should be opened in a separate browser window when user has a valid session token on the Neon platform</t>
   </si>
 </sst>
 </file>
@@ -409,7 +413,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -444,7 +448,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -653,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1014,6 +1018,21 @@
         <v>52</v>
       </c>
       <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Added Customer care scripts for IPA
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IPAIAM.xlsx
+++ b/src/test/resources/xls/IPAIAM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="83">
   <si>
     <t>TCID</t>
   </si>
@@ -248,6 +248,33 @@
   </si>
   <si>
     <t>Verify that the new STeAM step up authentication modal should include a link to initiate the EndNote supported forgot password flow. || Verify that the "Sign in to Target Druggability" modal should match with wireframe || Verify that the target application product overview page should be opened in a separate browser window when User clicks "Learn more" in any of the Step up related messages/modals.||Verify that the DRA\IPA application overview page should be opened in a separate browser window when user has a valid session token on the Neon platform</t>
+  </si>
+  <si>
+    <t>IPAIAMCC001</t>
+  </si>
+  <si>
+    <t>OPQA-5169||OPQA-5170</t>
+  </si>
+  <si>
+    <t>IPAIAMCC002</t>
+  </si>
+  <si>
+    <t>Verify that error messages/validation alerts "Please enter at least 2 characters for name" should be displayed when 'name' field is empty or 'name' field contains less than two characters.||Verify that error messages/validation alerts "Please enter at least 2 characters for Organization Name " should be displayed when 'Organization Name' field is empty or 'Organization Name' field contains less than two characters.</t>
+  </si>
+  <si>
+    <t>OPQA-5171||OPQA-5172</t>
+  </si>
+  <si>
+    <t>Verify that error messages/validation alerts " Incorrect email address format. Please try again." should be displayed when user enters incorrect email address.||Verify that error messages/validation alerts "Incorrect phone number format. Please try again.." should be displayed when user enters incorrect phone number.</t>
+  </si>
+  <si>
+    <t>IPAIAMCC003</t>
+  </si>
+  <si>
+    <t>Verify that the user should be able to select the issue type/category of the issue as an option</t>
+  </si>
+  <si>
+    <t>OPQA-5174</t>
   </si>
 </sst>
 </file>
@@ -311,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -325,6 +352,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -657,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,7 +942,7 @@
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>50</v>
       </c>
@@ -929,7 +957,7 @@
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>51</v>
       </c>
@@ -944,7 +972,7 @@
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>54</v>
       </c>
@@ -959,7 +987,7 @@
       </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>59</v>
       </c>
@@ -974,7 +1002,7 @@
       </c>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>62</v>
       </c>
@@ -989,7 +1017,7 @@
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>63</v>
       </c>
@@ -1004,7 +1032,7 @@
       </c>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>70</v>
       </c>
@@ -1019,7 +1047,7 @@
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>71</v>
       </c>
@@ -1033,6 +1061,53 @@
         <v>52</v>
       </c>
       <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1041,6 +1116,7 @@
     <hyperlink ref="B8" r:id="rId3" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-4223"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added new customer care scripts for IPAIAM
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IPAIAM.xlsx
+++ b/src/test/resources/xls/IPAIAM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="92">
   <si>
     <t>TCID</t>
   </si>
@@ -284,6 +284,27 @@
   </si>
   <si>
     <t>Verify that Page should change header title for different title||Ensure that the page has "Support Request" and "Call us" sections.</t>
+  </si>
+  <si>
+    <t>OPQA-5154||OPQA-5230</t>
+  </si>
+  <si>
+    <t>Verify that a "Call us" section is present in customer care contact page with customer care contact details (region, phone numbers, hours of operation, language supported||Ensure that the page has "Support Request" and "Call us" sections.</t>
+  </si>
+  <si>
+    <t>OPQA-5168 || OPQA-5227</t>
+  </si>
+  <si>
+    <t>Verify that the web form provided to user should be application specific with following required fields
+1.Name 2.Organization 3.Contact details (email, telephone) 4.Issue Category 5.Country
+6.Description of issue ( a free form text box where a user can describe why they are contacting support) ||
+Verify that the web form provided to user will be application specific with following required fields (Name, Organization, email, telephone, Issue Category, Country, Description of issue)</t>
+  </si>
+  <si>
+    <t>IPAIAM070</t>
+  </si>
+  <si>
+    <t>IPAIAM071</t>
   </si>
 </sst>
 </file>
@@ -697,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1136,6 +1157,36 @@
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E30" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
commented IPAIAM appswitcher related script
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IPAIAM.xlsx
+++ b/src/test/resources/xls/IPAIAM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="93">
   <si>
     <t>TCID</t>
   </si>
@@ -305,6 +305,9 @@
   </si>
   <si>
     <t>IPAIAM071</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -720,8 +723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,7 +809,7 @@
         <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>52</v>
+        <v>92</v>
       </c>
       <c r="E5" s="2"/>
     </row>

</xml_diff>